<commit_message>
Add support for formula
</commit_message>
<xml_diff>
--- a/examples/output/set_background2.xlsx
+++ b/examples/output/set_background2.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -334,6 +334,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" ht="15">
+      <c r="A1" t="str">
+        <v>Sheet1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <picture r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="00000000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -347,23 +369,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <picture r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" ht="15">
-      <c r="A1" t="str">
-        <v>Sheet1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <picture r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>